<commit_message>
feat: Se arreglo la logica de departamentos y ais mismo la de usuarios se sigue realizando lo de administradores
</commit_message>
<xml_diff>
--- a/assets/plantillas/superadmin-condo-detallado-report.xlsx
+++ b/assets/plantillas/superadmin-condo-detallado-report.xlsx
@@ -20,17 +20,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Reporte Condominio Detallado</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre:  ${other.condominioNombre}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emitido: ${other.generationDate}</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nombre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  ${other.condominioNombre}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamentos:  ${other.totalDepartamentos}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Areas comunales:  ${other.areasComunes}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador:  ${other.admin}</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -55,25 +84,16 @@
     <t xml:space="preserve">Admin </t>
   </si>
   <si>
-    <t xml:space="preserve">Total Usuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N.° Torres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N.° Total Bloques de Casas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo Cond.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Identificador</t>
   </si>
   <si>
-    <t xml:space="preserve">Cantidad Casas por Bloque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Interno</t>
+    <t xml:space="preserve">Codigo departamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre departamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propietario</t>
   </si>
   <si>
     <t xml:space="preserve">${table:detalles.id}</t>
@@ -100,25 +120,19 @@
     <t xml:space="preserve">${table:detalles.admin}</t>
   </si>
   <si>
-    <t xml:space="preserve">${table:detalles.totalUsuarios}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:detalles.cantidadTorres}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:detalles.cantidadCasas}</t>
-  </si>
-  <si>
     <t xml:space="preserve">${table:detalles.identificador}</t>
   </si>
   <si>
-    <t xml:space="preserve">${table:detalles.cantidad}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:detalles.codigo}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${table:detalles.nombreUnidad}</t>
+    <t xml:space="preserve">${table:detalles.codigoDepartamento}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:detalles.nombreDepartamento}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:detalles.estadoDepartamento}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:detalles.propietario}</t>
   </si>
 </sst>
 </file>
@@ -128,7 +142,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -152,6 +166,14 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -231,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,11 +266,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,15 +528,15 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.9"/>
@@ -519,10 +545,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="30.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="20.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21.7"/>
@@ -533,120 +560,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0"/>
-    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="J12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="K12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="L12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="M12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="2" t="s">
+      <c r="O12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="O13" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>